<commit_message>
Rework escritura odt, odp, ods, y odg
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -24,9 +24,6 @@
     <t>pepe</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>cuadro</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>por</t>
+  </si>
+  <si>
+    <t>Amortización</t>
   </si>
 </sst>
 </file>
@@ -102,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,57 +407,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D6:J13"/>
+  <dimension ref="D5:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
@@ -470,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.25">
@@ -484,85 +488,85 @@
         <v>6</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentación + cambios al cambiar palabras
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16383" windowHeight="8192" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16383" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>pepe</t>
   </si>
@@ -43,9 +43,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -86,6 +83,15 @@
   </si>
   <si>
     <t>losa</t>
+  </si>
+  <si>
+    <t>c/\</t>
+  </si>
+  <si>
+    <t>a"\</t>
+  </si>
+  <si>
+    <t>s/</t>
   </si>
 </sst>
 </file>
@@ -428,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:J14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -448,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
         <v>3</v>
@@ -459,33 +465,33 @@
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="4:10" x14ac:dyDescent="0.25">
@@ -499,7 +505,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.25">
@@ -513,85 +519,85 @@
         <v>6</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
       </c>
       <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
         <v>13</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="4:10" x14ac:dyDescent="0.25">
@@ -609,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -617,15 +623,15 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -633,10 +639,10 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>